<commit_message>
version 30.08.24 part + admin
</commit_message>
<xml_diff>
--- a/users_data.xlsx
+++ b/users_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,22 +446,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>ИМЯ/First Name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>ФАМИЛИЯ/Last Name</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Username</t>
+          <t>ЛОГИН/Username</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>НОМЕР ТЕЛ./Phone</t>
         </is>
       </c>
     </row>
@@ -488,22 +488,6 @@
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>6625770047</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>kiper_slivki</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>